<commit_message>
changed csv file format
</commit_message>
<xml_diff>
--- a/data/4sensors/linear_data.xlsx
+++ b/data/4sensors/linear_data.xlsx
@@ -467,19 +467,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4920</v>
+        <v>644155.5325713719</v>
       </c>
       <c r="B2" t="n">
-        <v>-261.07</v>
+        <v>-297.4396929233496</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>66.9109211573209</v>
       </c>
       <c r="D2" t="n">
-        <v>-20.61</v>
+        <v>35.07948187746732</v>
       </c>
       <c r="E2" t="n">
-        <v>1019.165107608548</v>
+        <v>952.59816358545</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
@@ -487,99 +487,99 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>800</v>
+        <v>5043309.206599923</v>
       </c>
       <c r="B3" t="n">
-        <v>164.42</v>
+        <v>-255.1120381994348</v>
       </c>
       <c r="C3" t="n">
-        <v>-64.7</v>
+        <v>78.74441128961679</v>
       </c>
       <c r="D3" t="n">
-        <v>-36.2</v>
+        <v>54.5198292297277</v>
       </c>
       <c r="E3" t="n">
-        <v>830.5141707359672</v>
+        <v>924.4962212772796</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2911271.868968321</v>
+        <v>49186920.39333353</v>
       </c>
       <c r="B4" t="n">
-        <v>80.15108206975451</v>
+        <v>-85.83042780944994</v>
       </c>
       <c r="C4" t="n">
-        <v>-36.71586761817326</v>
+        <v>99.99335942450048</v>
       </c>
       <c r="D4" t="n">
-        <v>102.972045398455</v>
+        <v>61.6573218516203</v>
       </c>
       <c r="E4" t="n">
-        <v>504.7540199216184</v>
+        <v>893.3942691621802</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>5.348188706381166</v>
       </c>
       <c r="B5" t="n">
-        <v>166.657</v>
+        <v>-138.9661583473835</v>
       </c>
       <c r="C5" t="n">
-        <v>-68.8</v>
+        <v>-42.78194712302945</v>
       </c>
       <c r="D5" t="n">
-        <v>-56.36</v>
+        <v>-59.18489208057598</v>
       </c>
       <c r="E5" t="n">
-        <v>1096.089276117494</v>
+        <v>590.3910345024965</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4980412.217611824</v>
+        <v>800</v>
       </c>
       <c r="B6" t="n">
-        <v>-256.4562557870458</v>
+        <v>164.42</v>
       </c>
       <c r="C6" t="n">
-        <v>78.6937047261474</v>
+        <v>-64.7</v>
       </c>
       <c r="D6" t="n">
-        <v>54.80577586093764</v>
+        <v>-36.2</v>
       </c>
       <c r="E6" t="n">
-        <v>924.6675986086806</v>
+        <v>830.5141707359672</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>30684463.34313393</v>
+        <v>4040652.814391558</v>
       </c>
       <c r="B7" t="n">
-        <v>-68.21358474433076</v>
+        <v>-93.17534123531067</v>
       </c>
       <c r="C7" t="n">
-        <v>70.68786931589013</v>
+        <v>51.52290082809784</v>
       </c>
       <c r="D7" t="n">
-        <v>52.95135844927474</v>
+        <v>35.25046438314074</v>
       </c>
       <c r="E7" t="n">
-        <v>411.8155885141013</v>
+        <v>434.3821835375155</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -587,39 +587,39 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>49200000</v>
+        <v>3050</v>
       </c>
       <c r="B8" t="n">
-        <v>-84.64</v>
+        <v>-109.94</v>
       </c>
       <c r="C8" t="n">
-        <v>99.88</v>
+        <v>-19.62</v>
       </c>
       <c r="D8" t="n">
-        <v>61.648</v>
+        <v>-27.24</v>
       </c>
       <c r="E8" t="n">
-        <v>893.3906383471165</v>
+        <v>514.4037326287156</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>157.6768466409531</v>
+        <v>3227476.74352717</v>
       </c>
       <c r="B9" t="n">
-        <v>-114.249676540795</v>
+        <v>-95.30843533298756</v>
       </c>
       <c r="C9" t="n">
-        <v>-23.80164841421681</v>
+        <v>49.49104275998463</v>
       </c>
       <c r="D9" t="n">
-        <v>-34.69652084741048</v>
+        <v>32.2215445086691</v>
       </c>
       <c r="E9" t="n">
-        <v>547.3778756762034</v>
+        <v>436.8833996430057</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -627,59 +627,59 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1043823.4631708</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>-97.78949621847534</v>
+        <v>166.657</v>
       </c>
       <c r="C10" t="n">
-        <v>24.32618038631301</v>
+        <v>-68.8</v>
       </c>
       <c r="D10" t="n">
-        <v>16.00952962478613</v>
+        <v>-56.36</v>
       </c>
       <c r="E10" t="n">
-        <v>449.4482758226739</v>
+        <v>1096.089276117494</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3036921.674397244</v>
+        <v>30556.04118861206</v>
       </c>
       <c r="B11" t="n">
-        <v>-95.48484289643584</v>
+        <v>138.5510643468537</v>
       </c>
       <c r="C11" t="n">
-        <v>49.42245620892747</v>
+        <v>-60.11400736743543</v>
       </c>
       <c r="D11" t="n">
-        <v>33.21324102009174</v>
+        <v>28.35789161685785</v>
       </c>
       <c r="E11" t="n">
-        <v>437.5607952885894</v>
+        <v>685.7919250870542</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1200.893925373525</v>
+        <v>137053.563720391</v>
       </c>
       <c r="B12" t="n">
-        <v>-111.3750177120604</v>
+        <v>-99.88785680176473</v>
       </c>
       <c r="C12" t="n">
-        <v>-20.25328230894106</v>
+        <v>-0.1244350346787637</v>
       </c>
       <c r="D12" t="n">
-        <v>-29.77312923576422</v>
+        <v>-0.1543943636479058</v>
       </c>
       <c r="E12" t="n">
-        <v>524.7787372484659</v>
+        <v>472.0474142504115</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
@@ -687,39 +687,39 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>307452.0804862558</v>
+        <v>30774305.31316802</v>
       </c>
       <c r="B13" t="n">
-        <v>110.7449949234127</v>
+        <v>-67.92178603266238</v>
       </c>
       <c r="C13" t="n">
-        <v>-53.45362499009406</v>
+        <v>70.45670458141744</v>
       </c>
       <c r="D13" t="n">
-        <v>73.47481190751829</v>
+        <v>52.79954833614673</v>
       </c>
       <c r="E13" t="n">
-        <v>594.0665770416572</v>
+        <v>411.783045109778</v>
       </c>
       <c r="F13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>30291286.90646695</v>
+        <v>329549.1953043724</v>
       </c>
       <c r="B14" t="n">
-        <v>-67.97242965414624</v>
+        <v>-100.515817291604</v>
       </c>
       <c r="C14" t="n">
-        <v>71.21879167343796</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>52.5961963424289</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>411.9591386506028</v>
+        <v>462.2815195618131</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -727,59 +727,59 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>305000</v>
+        <v>328758.8362698939</v>
       </c>
       <c r="B15" t="n">
-        <v>-99.95999999999999</v>
+        <v>109.8612532923608</v>
       </c>
       <c r="C15" t="n">
-        <v>-8.390000000000001</v>
+        <v>-53.29187250986424</v>
       </c>
       <c r="D15" t="n">
-        <v>-10.41</v>
+        <v>74.35945868345271</v>
       </c>
       <c r="E15" t="n">
-        <v>463.1432194547415</v>
+        <v>591.4045048554999</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>280744.9702550099</v>
+        <v>157.6768466409531</v>
       </c>
       <c r="B16" t="n">
-        <v>109.9567891900773</v>
+        <v>-114.249676540795</v>
       </c>
       <c r="C16" t="n">
-        <v>-53.29471813686553</v>
+        <v>-23.80164841421681</v>
       </c>
       <c r="D16" t="n">
-        <v>74.32551204426061</v>
+        <v>-34.69652084741048</v>
       </c>
       <c r="E16" t="n">
-        <v>597.6768824721285</v>
+        <v>547.3778756762034</v>
       </c>
       <c r="F16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2911271.86896832</v>
+        <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>80.15108206975451</v>
+        <v>138.545990545099</v>
       </c>
       <c r="C17" t="n">
-        <v>-36.71586761817326</v>
+        <v>-59.89135840171184</v>
       </c>
       <c r="D17" t="n">
-        <v>102.972045398455</v>
+        <v>28.02298841894063</v>
       </c>
       <c r="E17" t="n">
-        <v>504.7540199216184</v>
+        <v>1096.089276117494</v>
       </c>
       <c r="F17" t="n">
         <v>3</v>
@@ -787,39 +787,39 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3331523.084618582</v>
+        <v>180</v>
       </c>
       <c r="B18" t="n">
-        <v>-95.58968015431776</v>
+        <v>-255.28</v>
       </c>
       <c r="C18" t="n">
-        <v>49.63611264256301</v>
+        <v>5</v>
       </c>
       <c r="D18" t="n">
-        <v>33.58881209296357</v>
+        <v>-26.12</v>
       </c>
       <c r="E18" t="n">
-        <v>436.5302222583106</v>
+        <v>1064.339919849303</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>80.14117124951717</v>
+        <v>30291286.90646695</v>
       </c>
       <c r="B19" t="n">
-        <v>-115.1775826250006</v>
+        <v>-67.97242965414624</v>
       </c>
       <c r="C19" t="n">
-        <v>-25.24623656817509</v>
+        <v>71.21879167343796</v>
       </c>
       <c r="D19" t="n">
-        <v>-36.26591143367618</v>
+        <v>52.5961963424289</v>
       </c>
       <c r="E19" t="n">
-        <v>554.9109218187826</v>
+        <v>411.9591386506028</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
@@ -827,79 +827,79 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>10</v>
+        <v>301670.6973956299</v>
       </c>
       <c r="B20" t="n">
-        <v>-128.55</v>
+        <v>-299.6207318655524</v>
       </c>
       <c r="C20" t="n">
-        <v>-35.58</v>
+        <v>66.61558663348526</v>
       </c>
       <c r="D20" t="n">
-        <v>-54.39</v>
+        <v>35.43260039756296</v>
       </c>
       <c r="E20" t="n">
-        <v>578.0769749501844</v>
+        <v>962.9575027203946</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>416345.7451870226</v>
+        <v>4429594.436841236</v>
       </c>
       <c r="B21" t="n">
-        <v>-100.1077717828337</v>
+        <v>-255.8077414015688</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>78.23075826685006</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>54.67402251073113</v>
       </c>
       <c r="E21" t="n">
-        <v>459.6791802865195</v>
+        <v>926.2681203853519</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>4303973.843162411</v>
+        <v>2911271.868968321</v>
       </c>
       <c r="B22" t="n">
-        <v>-258.6368853349424</v>
+        <v>80.15108206975451</v>
       </c>
       <c r="C22" t="n">
-        <v>78.61680679637722</v>
+        <v>-36.71586761817326</v>
       </c>
       <c r="D22" t="n">
-        <v>55.15542617608244</v>
+        <v>102.972045398455</v>
       </c>
       <c r="E22" t="n">
-        <v>926.6609876866456</v>
+        <v>504.7540199216184</v>
       </c>
       <c r="F22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>4648.67440764958</v>
       </c>
       <c r="B23" t="n">
-        <v>-183.78</v>
+        <v>-107.6411240982927</v>
       </c>
       <c r="C23" t="n">
-        <v>-65.5</v>
+        <v>-15.15492386055267</v>
       </c>
       <c r="D23" t="n">
-        <v>-68.34</v>
+        <v>-21.04078113972756</v>
       </c>
       <c r="E23" t="n">
-        <v>603.7072315371715</v>
+        <v>509.7126449633075</v>
       </c>
       <c r="F23" t="n">
         <v>1</v>
@@ -907,39 +907,39 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2880000</v>
+        <v>10</v>
       </c>
       <c r="B24" t="n">
-        <v>80.43000000000001</v>
+        <v>-128.55</v>
       </c>
       <c r="C24" t="n">
-        <v>-36.7</v>
+        <v>-35.58</v>
       </c>
       <c r="D24" t="n">
-        <v>102.4</v>
+        <v>-54.39</v>
       </c>
       <c r="E24" t="n">
-        <v>505.1830870831064</v>
+        <v>578.0769749501844</v>
       </c>
       <c r="F24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>4917315.128981112</v>
+        <v>4980412.217611824</v>
       </c>
       <c r="B25" t="n">
-        <v>-254.6292588979523</v>
+        <v>-256.4562557870458</v>
       </c>
       <c r="C25" t="n">
-        <v>78.42573861667788</v>
+        <v>78.6937047261474</v>
       </c>
       <c r="D25" t="n">
-        <v>54.9571417329734</v>
+        <v>54.80577586093764</v>
       </c>
       <c r="E25" t="n">
-        <v>924.8417097358416</v>
+        <v>924.6675986086806</v>
       </c>
       <c r="F25" t="n">
         <v>2</v>
@@ -947,19 +947,19 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>30774305.31316798</v>
+        <v>700</v>
       </c>
       <c r="B26" t="n">
-        <v>-67.92178603266238</v>
+        <v>-112.206</v>
       </c>
       <c r="C26" t="n">
-        <v>70.45670458141744</v>
+        <v>-20.62</v>
       </c>
       <c r="D26" t="n">
-        <v>52.79954833614673</v>
+        <v>-31.24</v>
       </c>
       <c r="E26" t="n">
-        <v>411.783045109778</v>
+        <v>530.7866387564721</v>
       </c>
       <c r="F26" t="n">
         <v>1</v>
@@ -967,19 +967,19 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>490</v>
+        <v>4303973.843162411</v>
       </c>
       <c r="B27" t="n">
-        <v>-252.281</v>
+        <v>-258.6368853349424</v>
       </c>
       <c r="C27" t="n">
-        <v>3</v>
+        <v>78.61680679637722</v>
       </c>
       <c r="D27" t="n">
-        <v>-22.08</v>
+        <v>55.15542617608244</v>
       </c>
       <c r="E27" t="n">
-        <v>1050.664349397928</v>
+        <v>926.6609876866456</v>
       </c>
       <c r="F27" t="n">
         <v>2</v>
@@ -987,19 +987,19 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>4040652.814391558</v>
+        <v>9146.214239576677</v>
       </c>
       <c r="B28" t="n">
-        <v>-93.17534123531067</v>
+        <v>-103.9495413612393</v>
       </c>
       <c r="C28" t="n">
-        <v>51.52290082809784</v>
+        <v>-7.984811727152668</v>
       </c>
       <c r="D28" t="n">
-        <v>35.25046438314074</v>
+        <v>-11.08594655696425</v>
       </c>
       <c r="E28" t="n">
-        <v>434.3821835375155</v>
+        <v>502.1795988207282</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
@@ -1007,79 +1007,79 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>644155.5325713719</v>
+        <v>305000</v>
       </c>
       <c r="B29" t="n">
-        <v>-297.4396929233496</v>
+        <v>-99.95999999999999</v>
       </c>
       <c r="C29" t="n">
-        <v>66.9109211573209</v>
+        <v>-8.390000000000001</v>
       </c>
       <c r="D29" t="n">
-        <v>35.07948187746732</v>
+        <v>-10.41</v>
       </c>
       <c r="E29" t="n">
-        <v>952.59816358545</v>
+        <v>463.1432194547415</v>
       </c>
       <c r="F29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>3050000</v>
+        <v>2880</v>
       </c>
       <c r="B30" t="n">
-        <v>-95.7</v>
+        <v>161.443</v>
       </c>
       <c r="C30" t="n">
-        <v>50.162</v>
+        <v>-62.8</v>
       </c>
       <c r="D30" t="n">
-        <v>32.63</v>
+        <v>25.4</v>
       </c>
       <c r="E30" t="n">
-        <v>437.5129628677545</v>
+        <v>779.6235349212776</v>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>40376.2137451594</v>
+        <v>2362.745195146051</v>
       </c>
       <c r="B31" t="n">
-        <v>138.7625648348168</v>
+        <v>-110.3330851986241</v>
       </c>
       <c r="C31" t="n">
-        <v>-60.17878747169322</v>
+        <v>-19.79347096144048</v>
       </c>
       <c r="D31" t="n">
-        <v>27.41091523539398</v>
+        <v>-27.93388384576191</v>
       </c>
       <c r="E31" t="n">
-        <v>674.7202194699697</v>
+        <v>517.2456911058866</v>
       </c>
       <c r="F31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7949938.642155684</v>
+        <v>1043823.4631708</v>
       </c>
       <c r="B32" t="n">
-        <v>-84.70839587504587</v>
+        <v>-97.78949621847534</v>
       </c>
       <c r="C32" t="n">
-        <v>58.13975662557907</v>
+        <v>24.32618038631301</v>
       </c>
       <c r="D32" t="n">
-        <v>41.07778176510754</v>
+        <v>16.00952962478613</v>
       </c>
       <c r="E32" t="n">
-        <v>426.8491373949363</v>
+        <v>449.4482758226739</v>
       </c>
       <c r="F32" t="n">
         <v>1</v>
@@ -1087,19 +1087,19 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1</v>
+        <v>1124994.013311719</v>
       </c>
       <c r="B33" t="n">
-        <v>-131.26</v>
+        <v>-295.9460021527</v>
       </c>
       <c r="C33" t="n">
-        <v>45.31</v>
+        <v>66.62874935399593</v>
       </c>
       <c r="D33" t="n">
-        <v>-69</v>
+        <v>35.64750073371923</v>
       </c>
       <c r="E33" t="n">
-        <v>1135.25384544162</v>
+        <v>944.9837938784092</v>
       </c>
       <c r="F33" t="n">
         <v>2</v>
@@ -1107,22 +1107,22 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>19433.41874380765</v>
+        <v>288000</v>
       </c>
       <c r="B34" t="n">
-        <v>-99.8385047997232</v>
+        <v>109.723</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>-53.4</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>73.8</v>
       </c>
       <c r="E34" t="n">
-        <v>493.7906149301896</v>
+        <v>596.6632363624968</v>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -1130,76 +1130,76 @@
         <v>1</v>
       </c>
       <c r="B35" t="n">
-        <v>-150.23</v>
+        <v>-137.72</v>
       </c>
       <c r="C35" t="n">
-        <v>-50.57</v>
+        <v>35.203</v>
       </c>
       <c r="D35" t="n">
-        <v>-64.37</v>
+        <v>-34.81</v>
       </c>
       <c r="E35" t="n">
-        <v>603.7072315371715</v>
+        <v>1135.25384544162</v>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>20</v>
+        <v>1200.893925373525</v>
       </c>
       <c r="B36" t="n">
-        <v>165</v>
+        <v>-111.3750177120604</v>
       </c>
       <c r="C36" t="n">
-        <v>-68.3</v>
+        <v>-20.25328230894106</v>
       </c>
       <c r="D36" t="n">
-        <v>-54.59</v>
+        <v>-29.77312923576422</v>
       </c>
       <c r="E36" t="n">
-        <v>977.070857897188</v>
+        <v>524.7787372484659</v>
       </c>
       <c r="F36" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>30500000</v>
+        <v>2843404.369240924</v>
       </c>
       <c r="B37" t="n">
-        <v>-68.02</v>
+        <v>79.430555865225</v>
       </c>
       <c r="C37" t="n">
-        <v>70.73399999999999</v>
+        <v>-36.57172150508754</v>
       </c>
       <c r="D37" t="n">
-        <v>52.47</v>
+        <v>103.484187598182</v>
       </c>
       <c r="E37" t="n">
-        <v>411.8827062807674</v>
+        <v>505.6911551465355</v>
       </c>
       <c r="F37" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>30500</v>
+        <v>7949938.642155684</v>
       </c>
       <c r="B38" t="n">
-        <v>-107.42</v>
+        <v>-84.70839587504587</v>
       </c>
       <c r="C38" t="n">
-        <v>-18.7</v>
+        <v>58.13975662557907</v>
       </c>
       <c r="D38" t="n">
-        <v>-23.93</v>
+        <v>41.07778176510754</v>
       </c>
       <c r="E38" t="n">
-        <v>488.7734760417285</v>
+        <v>426.8491373949363</v>
       </c>
       <c r="F38" t="n">
         <v>1</v>
@@ -1207,10 +1207,10 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>135412.953500118</v>
+        <v>19433.41874380765</v>
       </c>
       <c r="B39" t="n">
-        <v>-99.88677071250018</v>
+        <v>-99.8385047997232</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>472.18146362185</v>
+        <v>493.7906149301896</v>
       </c>
       <c r="F39" t="n">
         <v>1</v>
@@ -1227,79 +1227,79 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>610.3689144990043</v>
+        <v>1</v>
       </c>
       <c r="B40" t="n">
-        <v>-112.3938643723838</v>
+        <v>-131.26</v>
       </c>
       <c r="C40" t="n">
-        <v>-20.91247210630024</v>
+        <v>45.31</v>
       </c>
       <c r="D40" t="n">
-        <v>-31.55773967487909</v>
+        <v>-69</v>
       </c>
       <c r="E40" t="n">
-        <v>532.3117833910451</v>
+        <v>1135.25384544162</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2695592.704856827</v>
+        <v>49954514.14071552</v>
       </c>
       <c r="B41" t="n">
-        <v>-95.39656680593912</v>
+        <v>-85.51930502846753</v>
       </c>
       <c r="C41" t="n">
-        <v>49.43572018219157</v>
+        <v>99.83840661971864</v>
       </c>
       <c r="D41" t="n">
-        <v>32.534603222162</v>
+        <v>61.32875775302923</v>
       </c>
       <c r="E41" t="n">
-        <v>438.8879125143717</v>
+        <v>893.1828074633391</v>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0</v>
+        <v>48933670.71017869</v>
       </c>
       <c r="B42" t="n">
-        <v>138.545990545099</v>
+        <v>-87.55090948856086</v>
       </c>
       <c r="C42" t="n">
-        <v>-59.89135840171184</v>
+        <v>100.119234532258</v>
       </c>
       <c r="D42" t="n">
-        <v>28.02298841894063</v>
+        <v>61.84352461305254</v>
       </c>
       <c r="E42" t="n">
-        <v>1096.089276117494</v>
+        <v>893.4647606258434</v>
       </c>
       <c r="F42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>5.348188706381166</v>
+        <v>80.14117124951717</v>
       </c>
       <c r="B43" t="n">
-        <v>-138.9661583473835</v>
+        <v>-115.1775826250006</v>
       </c>
       <c r="C43" t="n">
-        <v>-42.78194712302945</v>
+        <v>-25.24623656817509</v>
       </c>
       <c r="D43" t="n">
-        <v>-59.18489208057598</v>
+        <v>-36.26591143367618</v>
       </c>
       <c r="E43" t="n">
-        <v>590.3910345024965</v>
+        <v>554.9109218187826</v>
       </c>
       <c r="F43" t="n">
         <v>1</v>
@@ -1307,79 +1307,79 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>48933670.71017869</v>
+        <v>279328.569773039</v>
       </c>
       <c r="B44" t="n">
-        <v>-87.55090948856086</v>
+        <v>108.8274212357594</v>
       </c>
       <c r="C44" t="n">
-        <v>100.119234532258</v>
+        <v>-53.15930070178533</v>
       </c>
       <c r="D44" t="n">
-        <v>61.84352461305254</v>
+        <v>74.35786179738852</v>
       </c>
       <c r="E44" t="n">
-        <v>893.4647606258434</v>
+        <v>597.8778302036573</v>
       </c>
       <c r="F44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>310.2274096946697</v>
+        <v>492000</v>
       </c>
       <c r="B45" t="n">
-        <v>-113.3217704565894</v>
+        <v>-298.65</v>
       </c>
       <c r="C45" t="n">
-        <v>-22.35706026025852</v>
+        <v>66.63</v>
       </c>
       <c r="D45" t="n">
-        <v>-33.12713026114479</v>
+        <v>35.35</v>
       </c>
       <c r="E45" t="n">
-        <v>539.8448295336242</v>
+        <v>956.277872977832</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>30556.04118861206</v>
+        <v>2695592.704856827</v>
       </c>
       <c r="B46" t="n">
-        <v>138.5510643468537</v>
+        <v>-95.39656680593912</v>
       </c>
       <c r="C46" t="n">
-        <v>-60.11400736743543</v>
+        <v>49.43572018219157</v>
       </c>
       <c r="D46" t="n">
-        <v>28.35789161685785</v>
+        <v>32.534603222162</v>
       </c>
       <c r="E46" t="n">
-        <v>685.7919250870542</v>
+        <v>438.8879125143717</v>
       </c>
       <c r="F46" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0</v>
+        <v>48585266.5503143</v>
       </c>
       <c r="B47" t="n">
-        <v>-297.7465279776833</v>
+        <v>-81.7078693439482</v>
       </c>
       <c r="C47" t="n">
-        <v>66.70701860920806</v>
+        <v>100.2812236660623</v>
       </c>
       <c r="D47" t="n">
-        <v>35.16125023638222</v>
+        <v>61.79521468432186</v>
       </c>
       <c r="E47" t="n">
-        <v>1135.25384544162</v>
+        <v>893.5623366298774</v>
       </c>
       <c r="F47" t="n">
         <v>2</v>
@@ -1387,19 +1387,19 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>137053.563720391</v>
+        <v>17995.07291338374</v>
       </c>
       <c r="B48" t="n">
-        <v>-99.88785680176473</v>
+        <v>-100.257958624186</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.1244350346787637</v>
+        <v>-0.8146995937526675</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.1543943636479058</v>
+        <v>-1.131111974200952</v>
       </c>
       <c r="E48" t="n">
-        <v>472.0474142504115</v>
+        <v>494.6465526781491</v>
       </c>
       <c r="F48" t="n">
         <v>1</v>
@@ -1407,19 +1407,19 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>49200</v>
+        <v>4920000</v>
       </c>
       <c r="B49" t="n">
-        <v>-277.04</v>
+        <v>-255.56</v>
       </c>
       <c r="C49" t="n">
-        <v>13</v>
+        <v>78.77</v>
       </c>
       <c r="D49" t="n">
-        <v>-4.65</v>
+        <v>54.62</v>
       </c>
       <c r="E49" t="n">
-        <v>987.7214902931898</v>
+        <v>924.8342556624744</v>
       </c>
       <c r="F49" t="n">
         <v>2</v>
@@ -1427,119 +1427,119 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>9146.214239576677</v>
+        <v>0</v>
       </c>
       <c r="B50" t="n">
-        <v>-103.9495413612393</v>
+        <v>-297.7465279776833</v>
       </c>
       <c r="C50" t="n">
-        <v>-7.984811727152668</v>
+        <v>66.70701860920806</v>
       </c>
       <c r="D50" t="n">
-        <v>-11.08594655696425</v>
+        <v>35.16125023638222</v>
       </c>
       <c r="E50" t="n">
-        <v>502.1795988207282</v>
+        <v>1135.25384544162</v>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>69659.13737153406</v>
+        <v>20</v>
       </c>
       <c r="B51" t="n">
-        <v>-103.2461184374148</v>
+        <v>165</v>
       </c>
       <c r="C51" t="n">
-        <v>-8.339027004015671</v>
+        <v>-68.3</v>
       </c>
       <c r="D51" t="n">
-        <v>-10.67127894150241</v>
+        <v>-54.59</v>
       </c>
       <c r="E51" t="n">
-        <v>479.5804603929906</v>
+        <v>977.070857897188</v>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1124994.013311719</v>
+        <v>3036921.674397244</v>
       </c>
       <c r="B52" t="n">
-        <v>-295.9460021527</v>
+        <v>-95.48484289643584</v>
       </c>
       <c r="C52" t="n">
-        <v>66.62874935399593</v>
+        <v>49.42245620892747</v>
       </c>
       <c r="D52" t="n">
-        <v>35.64750073371923</v>
+        <v>33.21324102009174</v>
       </c>
       <c r="E52" t="n">
-        <v>944.9837938784092</v>
+        <v>437.5607952885894</v>
       </c>
       <c r="F52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2880</v>
+        <v>269651.3341569912</v>
       </c>
       <c r="B53" t="n">
-        <v>161.443</v>
+        <v>-99.94889073617998</v>
       </c>
       <c r="C53" t="n">
-        <v>-62.8</v>
+        <v>-7.117193358938424</v>
       </c>
       <c r="D53" t="n">
-        <v>25.4</v>
+        <v>-8.830748851793684</v>
       </c>
       <c r="E53" t="n">
-        <v>779.6235349212776</v>
+        <v>464.5143681078323</v>
       </c>
       <c r="F53" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>80</v>
+        <v>2894954.494053226</v>
       </c>
       <c r="B54" t="n">
-        <v>-115.18</v>
+        <v>80.36634729822217</v>
       </c>
       <c r="C54" t="n">
-        <v>-25.25</v>
+        <v>-36.36523016904646</v>
       </c>
       <c r="D54" t="n">
-        <v>-36.27</v>
+        <v>103.2442241350995</v>
       </c>
       <c r="E54" t="n">
-        <v>554.9305468624422</v>
+        <v>504.9773250225817</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>530535.9455007528</v>
+        <v>35405.10211938623</v>
       </c>
       <c r="B55" t="n">
-        <v>-99.49644958308151</v>
+        <v>-106.6663282582184</v>
       </c>
       <c r="C55" t="n">
-        <v>6.414739616791655</v>
+        <v>-16.82913412914416</v>
       </c>
       <c r="D55" t="n">
-        <v>4.221664161797348</v>
+        <v>-21.53589196312405</v>
       </c>
       <c r="E55" t="n">
-        <v>456.9813219652531</v>
+        <v>487.1135065355699</v>
       </c>
       <c r="F55" t="n">
         <v>1</v>
@@ -1547,59 +1547,59 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>10.52250069864085</v>
+        <v>2880000</v>
       </c>
       <c r="B56" t="n">
-        <v>-128.2225348049704</v>
+        <v>80.43000000000001</v>
       </c>
       <c r="C56" t="n">
-        <v>-35.32699211184324</v>
+        <v>-36.7</v>
       </c>
       <c r="D56" t="n">
-        <v>-53.94619526298156</v>
+        <v>102.4</v>
       </c>
       <c r="E56" t="n">
-        <v>577.5100602465202</v>
+        <v>505.1830870831064</v>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>3094890.507590655</v>
+        <v>280744.9702550099</v>
       </c>
       <c r="B57" t="n">
-        <v>-95.6594348389487</v>
+        <v>109.9567891900773</v>
       </c>
       <c r="C57" t="n">
-        <v>50.31631105325295</v>
+        <v>-53.29471813686553</v>
       </c>
       <c r="D57" t="n">
-        <v>32.35447316735974</v>
+        <v>74.32551204426061</v>
       </c>
       <c r="E57" t="n">
-        <v>437.3503273658779</v>
+        <v>597.6768824721285</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2362.745195146051</v>
+        <v>610.3689144990043</v>
       </c>
       <c r="B58" t="n">
-        <v>-110.3330851986241</v>
+        <v>-112.3938643723838</v>
       </c>
       <c r="C58" t="n">
-        <v>-19.79347096144048</v>
+        <v>-20.91247210630024</v>
       </c>
       <c r="D58" t="n">
-        <v>-27.93388384576191</v>
+        <v>-31.55773967487909</v>
       </c>
       <c r="E58" t="n">
-        <v>517.2456911058866</v>
+        <v>532.3117833910451</v>
       </c>
       <c r="F58" t="n">
         <v>1</v>
@@ -1607,39 +1607,39 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>274574.2547322999</v>
+        <v>324879.1482733022</v>
       </c>
       <c r="B59" t="n">
-        <v>109.0976284336094</v>
+        <v>-100.0577265614921</v>
       </c>
       <c r="C59" t="n">
-        <v>-53.58970016175422</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>74.03673858345766</v>
+        <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>598.5598645001678</v>
+        <v>462.4403865955508</v>
       </c>
       <c r="F59" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>328758.8362698939</v>
+        <v>38148.56238884891</v>
       </c>
       <c r="B60" t="n">
-        <v>109.8612532923608</v>
+        <v>138.579495932181</v>
       </c>
       <c r="C60" t="n">
-        <v>-53.29187250986424</v>
+        <v>-60.08818356139495</v>
       </c>
       <c r="D60" t="n">
-        <v>74.35945868345271</v>
+        <v>27.36802890149941</v>
       </c>
       <c r="E60" t="n">
-        <v>591.4045048554999</v>
+        <v>676.9749686192322</v>
       </c>
       <c r="F60" t="n">
         <v>3</v>
@@ -1647,79 +1647,79 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>288000</v>
+        <v>310.2274096946697</v>
       </c>
       <c r="B61" t="n">
-        <v>109.723</v>
+        <v>-113.3217704565894</v>
       </c>
       <c r="C61" t="n">
-        <v>-53.4</v>
+        <v>-22.35706026025852</v>
       </c>
       <c r="D61" t="n">
-        <v>73.8</v>
+        <v>-33.12713026114479</v>
       </c>
       <c r="E61" t="n">
-        <v>596.6632363624968</v>
+        <v>539.8448295336242</v>
       </c>
       <c r="F61" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1</v>
+        <v>30500</v>
       </c>
       <c r="B62" t="n">
-        <v>-137.72</v>
+        <v>-107.42</v>
       </c>
       <c r="C62" t="n">
-        <v>35.203</v>
+        <v>-18.7</v>
       </c>
       <c r="D62" t="n">
-        <v>-34.81</v>
+        <v>-23.93</v>
       </c>
       <c r="E62" t="n">
-        <v>1135.25384544162</v>
+        <v>488.7734760417285</v>
       </c>
       <c r="F62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2882822.168529236</v>
+        <v>3050000</v>
       </c>
       <c r="B63" t="n">
-        <v>80.66367116761286</v>
+        <v>-95.7</v>
       </c>
       <c r="C63" t="n">
-        <v>-36.7564281141496</v>
+        <v>50.162</v>
       </c>
       <c r="D63" t="n">
-        <v>101.9386502785829</v>
+        <v>32.63</v>
       </c>
       <c r="E63" t="n">
-        <v>505.1441746011087</v>
+        <v>437.5129628677545</v>
       </c>
       <c r="F63" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>279328.569773039</v>
+        <v>2911271.86896832</v>
       </c>
       <c r="B64" t="n">
-        <v>108.8274212357594</v>
+        <v>80.15108206975451</v>
       </c>
       <c r="C64" t="n">
-        <v>-53.15930070178533</v>
+        <v>-36.71586761817326</v>
       </c>
       <c r="D64" t="n">
-        <v>74.35786179738852</v>
+        <v>102.972045398455</v>
       </c>
       <c r="E64" t="n">
-        <v>597.8778302036573</v>
+        <v>504.7540199216184</v>
       </c>
       <c r="F64" t="n">
         <v>3</v>
@@ -1727,59 +1727,59 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>49954514.14071549</v>
+        <v>1</v>
       </c>
       <c r="B65" t="n">
-        <v>-85.51930502846753</v>
+        <v>-150.23</v>
       </c>
       <c r="C65" t="n">
-        <v>99.83840661971864</v>
+        <v>-50.57</v>
       </c>
       <c r="D65" t="n">
-        <v>61.32875775302923</v>
+        <v>-64.37</v>
       </c>
       <c r="E65" t="n">
-        <v>893.1828074633391</v>
+        <v>603.7072315371715</v>
       </c>
       <c r="F65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>324879.1482733022</v>
+        <v>28800</v>
       </c>
       <c r="B66" t="n">
-        <v>-100.0577265614921</v>
+        <v>139.061</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>-60.1</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>28.14</v>
       </c>
       <c r="E66" t="n">
-        <v>462.4403865955508</v>
+        <v>688.1433856418872</v>
       </c>
       <c r="F66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>4648.67440764958</v>
+        <v>30774305.31316798</v>
       </c>
       <c r="B67" t="n">
-        <v>-107.6411240982927</v>
+        <v>-67.92178603266238</v>
       </c>
       <c r="C67" t="n">
-        <v>-15.15492386055267</v>
+        <v>70.45670458141744</v>
       </c>
       <c r="D67" t="n">
-        <v>-21.04078113972756</v>
+        <v>52.79954833614673</v>
       </c>
       <c r="E67" t="n">
-        <v>509.7126449633075</v>
+        <v>411.783045109778</v>
       </c>
       <c r="F67" t="n">
         <v>1</v>
@@ -1787,19 +1787,19 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>40</v>
+        <v>49200000</v>
       </c>
       <c r="B68" t="n">
-        <v>-161.09</v>
+        <v>-84.64</v>
       </c>
       <c r="C68" t="n">
-        <v>6</v>
+        <v>99.88</v>
       </c>
       <c r="D68" t="n">
-        <v>-28.53</v>
+        <v>61.648</v>
       </c>
       <c r="E68" t="n">
-        <v>1084.879284158058</v>
+        <v>893.3906383471165</v>
       </c>
       <c r="F68" t="n">
         <v>2</v>
@@ -1807,39 +1807,39 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>4429594.436841236</v>
+        <v>69659.13737153406</v>
       </c>
       <c r="B69" t="n">
-        <v>-255.8077414015688</v>
+        <v>-103.2461184374148</v>
       </c>
       <c r="C69" t="n">
-        <v>78.23075826685006</v>
+        <v>-8.339027004015671</v>
       </c>
       <c r="D69" t="n">
-        <v>54.67402251073113</v>
+        <v>-10.67127894150241</v>
       </c>
       <c r="E69" t="n">
-        <v>926.2681203853519</v>
+        <v>479.5804603929906</v>
       </c>
       <c r="F69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2868522.534712504</v>
+        <v>1</v>
       </c>
       <c r="B70" t="n">
-        <v>80.0474108784976</v>
+        <v>167</v>
       </c>
       <c r="C70" t="n">
-        <v>-36.70771849049878</v>
+        <v>-69.56</v>
       </c>
       <c r="D70" t="n">
-        <v>103.631474908098</v>
+        <v>-67.8</v>
       </c>
       <c r="E70" t="n">
-        <v>505.3417339495609</v>
+        <v>1096.089276117494</v>
       </c>
       <c r="F70" t="n">
         <v>3</v>
@@ -1847,39 +1847,39 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>49954514.14071552</v>
+        <v>3331523.084618582</v>
       </c>
       <c r="B71" t="n">
-        <v>-85.51930502846753</v>
+        <v>-95.58968015431776</v>
       </c>
       <c r="C71" t="n">
-        <v>99.83840661971864</v>
+        <v>49.63611264256301</v>
       </c>
       <c r="D71" t="n">
-        <v>61.32875775302923</v>
+        <v>33.58881209296357</v>
       </c>
       <c r="E71" t="n">
-        <v>893.1828074633391</v>
+        <v>436.5302222583106</v>
       </c>
       <c r="F71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>30413290.45028438</v>
+        <v>15641414.22617057</v>
       </c>
       <c r="B72" t="n">
-        <v>-68.30186025811477</v>
+        <v>-76.24145051478104</v>
       </c>
       <c r="C72" t="n">
-        <v>71.5478840756502</v>
+        <v>64.7566124230603</v>
       </c>
       <c r="D72" t="n">
-        <v>53.67604158442349</v>
+        <v>46.90509914707435</v>
       </c>
       <c r="E72" t="n">
-        <v>411.9143962943325</v>
+        <v>419.3160912523571</v>
       </c>
       <c r="F72" t="n">
         <v>1</v>
@@ -1887,19 +1887,19 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>3227476.74352717</v>
+        <v>2053710.839964827</v>
       </c>
       <c r="B73" t="n">
-        <v>-95.30843533298756</v>
+        <v>-96.08254285386914</v>
       </c>
       <c r="C73" t="n">
-        <v>49.49104275998463</v>
+        <v>42.2376211558344</v>
       </c>
       <c r="D73" t="n">
-        <v>32.2215445086691</v>
+        <v>27.79739508777493</v>
       </c>
       <c r="E73" t="n">
-        <v>436.8833996430057</v>
+        <v>441.9152296800947</v>
       </c>
       <c r="F73" t="n">
         <v>1</v>
@@ -1907,59 +1907,59 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>269651.3341569912</v>
+        <v>2868522.534712504</v>
       </c>
       <c r="B74" t="n">
-        <v>-99.94889073617998</v>
+        <v>80.0474108784976</v>
       </c>
       <c r="C74" t="n">
-        <v>-7.117193358938424</v>
+        <v>-36.70771849049878</v>
       </c>
       <c r="D74" t="n">
-        <v>-8.830748851793684</v>
+        <v>103.631474908098</v>
       </c>
       <c r="E74" t="n">
-        <v>464.5143681078323</v>
+        <v>505.3417339495609</v>
       </c>
       <c r="F74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>301670.6973956299</v>
+        <v>307452.0804862558</v>
       </c>
       <c r="B75" t="n">
-        <v>-299.6207318655524</v>
+        <v>110.7449949234127</v>
       </c>
       <c r="C75" t="n">
-        <v>66.61558663348526</v>
+        <v>-53.45362499009406</v>
       </c>
       <c r="D75" t="n">
-        <v>35.43260039756296</v>
+        <v>73.47481190751829</v>
       </c>
       <c r="E75" t="n">
-        <v>962.9575027203946</v>
+        <v>594.0665770416572</v>
       </c>
       <c r="F75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>48585266.5503143</v>
+        <v>49200</v>
       </c>
       <c r="B76" t="n">
-        <v>-81.7078693439482</v>
+        <v>-277.04</v>
       </c>
       <c r="C76" t="n">
-        <v>100.2812236660623</v>
+        <v>13</v>
       </c>
       <c r="D76" t="n">
-        <v>61.79521468432186</v>
+        <v>-4.65</v>
       </c>
       <c r="E76" t="n">
-        <v>893.5623366298774</v>
+        <v>987.7214902931898</v>
       </c>
       <c r="F76" t="n">
         <v>2</v>
@@ -1967,19 +1967,19 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2053710.839964827</v>
+        <v>20.70290093182177</v>
       </c>
       <c r="B77" t="n">
-        <v>-96.08254285386914</v>
+        <v>-123.8712445521292</v>
       </c>
       <c r="C77" t="n">
-        <v>42.2376211558344</v>
+        <v>-31.96507525979762</v>
       </c>
       <c r="D77" t="n">
-        <v>27.79739508777493</v>
+        <v>-48.04900907139718</v>
       </c>
       <c r="E77" t="n">
-        <v>441.9152296800947</v>
+        <v>569.977014103941</v>
       </c>
       <c r="F77" t="n">
         <v>1</v>
@@ -1987,19 +1987,19 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>28800</v>
+        <v>40830.97717635731</v>
       </c>
       <c r="B78" t="n">
-        <v>139.061</v>
+        <v>138.875514995292</v>
       </c>
       <c r="C78" t="n">
-        <v>-60.1</v>
+        <v>-60.33794706532451</v>
       </c>
       <c r="D78" t="n">
-        <v>28.14</v>
+        <v>28.89648062289801</v>
       </c>
       <c r="E78" t="n">
-        <v>688.1433856418872</v>
+        <v>674.275243295229</v>
       </c>
       <c r="F78" t="n">
         <v>3</v>
@@ -2007,19 +2007,19 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>4920000</v>
+        <v>40</v>
       </c>
       <c r="B79" t="n">
-        <v>-255.56</v>
+        <v>-161.09</v>
       </c>
       <c r="C79" t="n">
-        <v>78.77</v>
+        <v>6</v>
       </c>
       <c r="D79" t="n">
-        <v>54.62</v>
+        <v>-28.53</v>
       </c>
       <c r="E79" t="n">
-        <v>924.8342556624744</v>
+        <v>1084.879284158058</v>
       </c>
       <c r="F79" t="n">
         <v>2</v>
@@ -2027,82 +2027,82 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>160</v>
+        <v>49954514.14071549</v>
       </c>
       <c r="B80" t="n">
-        <v>164.52</v>
+        <v>-85.51930502846753</v>
       </c>
       <c r="C80" t="n">
-        <v>-66.8</v>
+        <v>99.83840661971864</v>
       </c>
       <c r="D80" t="n">
-        <v>-56.61</v>
+        <v>61.32875775302923</v>
       </c>
       <c r="E80" t="n">
-        <v>894.4560510744424</v>
+        <v>893.1828074633391</v>
       </c>
       <c r="F80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>38148.56238884891</v>
+        <v>30413290.45028438</v>
       </c>
       <c r="B81" t="n">
-        <v>138.579495932181</v>
+        <v>-68.30186025811477</v>
       </c>
       <c r="C81" t="n">
-        <v>-60.08818356139495</v>
+        <v>71.5478840756502</v>
       </c>
       <c r="D81" t="n">
-        <v>27.36802890149941</v>
+        <v>53.67604158442349</v>
       </c>
       <c r="E81" t="n">
-        <v>676.9749686192322</v>
+        <v>411.9143962943325</v>
       </c>
       <c r="F81" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>49186920.39333353</v>
+        <v>135412.953500118</v>
       </c>
       <c r="B82" t="n">
-        <v>-85.83042780944994</v>
+        <v>-99.88677071250018</v>
       </c>
       <c r="C82" t="n">
-        <v>99.99335942450048</v>
+        <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>61.6573218516203</v>
+        <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>893.3942691621802</v>
+        <v>472.18146362185</v>
       </c>
       <c r="F82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>492000</v>
+        <v>40376.2137451594</v>
       </c>
       <c r="B83" t="n">
-        <v>-298.65</v>
+        <v>138.7625648348168</v>
       </c>
       <c r="C83" t="n">
-        <v>66.63</v>
+        <v>-60.17878747169322</v>
       </c>
       <c r="D83" t="n">
-        <v>35.35</v>
+        <v>27.41091523539398</v>
       </c>
       <c r="E83" t="n">
-        <v>956.277872977832</v>
+        <v>674.7202194699697</v>
       </c>
       <c r="F83" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
@@ -2127,19 +2127,19 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="B85" t="n">
-        <v>167</v>
+        <v>164.78</v>
       </c>
       <c r="C85" t="n">
-        <v>-69.56</v>
+        <v>-68</v>
       </c>
       <c r="D85" t="n">
-        <v>-67.8</v>
+        <v>-54.59</v>
       </c>
       <c r="E85" t="n">
-        <v>1096.089276117494</v>
+        <v>933.4237342910632</v>
       </c>
       <c r="F85" t="n">
         <v>3</v>
@@ -2147,79 +2147,79 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>5043309.206599923</v>
+        <v>274574.2547322999</v>
       </c>
       <c r="B86" t="n">
-        <v>-255.1120381994348</v>
+        <v>109.0976284336094</v>
       </c>
       <c r="C86" t="n">
-        <v>78.74441128961679</v>
+        <v>-53.58970016175422</v>
       </c>
       <c r="D86" t="n">
-        <v>54.5198292297277</v>
+        <v>74.03673858345766</v>
       </c>
       <c r="E86" t="n">
-        <v>924.4962212772796</v>
+        <v>598.5598645001678</v>
       </c>
       <c r="F86" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2894954.494053226</v>
+        <v>490</v>
       </c>
       <c r="B87" t="n">
-        <v>80.36634729822217</v>
+        <v>-252.281</v>
       </c>
       <c r="C87" t="n">
-        <v>-36.36523016904646</v>
+        <v>3</v>
       </c>
       <c r="D87" t="n">
-        <v>103.2442241350995</v>
+        <v>-22.08</v>
       </c>
       <c r="E87" t="n">
-        <v>504.9773250225817</v>
+        <v>1050.664349397928</v>
       </c>
       <c r="F87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>40830.97717635731</v>
+        <v>3094890.507590655</v>
       </c>
       <c r="B88" t="n">
-        <v>138.875514995292</v>
+        <v>-95.6594348389487</v>
       </c>
       <c r="C88" t="n">
-        <v>-60.33794706532451</v>
+        <v>50.31631105325295</v>
       </c>
       <c r="D88" t="n">
-        <v>28.89648062289801</v>
+        <v>32.35447316735974</v>
       </c>
       <c r="E88" t="n">
-        <v>674.275243295229</v>
+        <v>437.3503273658779</v>
       </c>
       <c r="F88" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>15641414.22617057</v>
+        <v>30684463.34313393</v>
       </c>
       <c r="B89" t="n">
-        <v>-76.24145051478104</v>
+        <v>-68.21358474433076</v>
       </c>
       <c r="C89" t="n">
-        <v>64.7566124230603</v>
+        <v>70.68786931589013</v>
       </c>
       <c r="D89" t="n">
-        <v>46.90509914707435</v>
+        <v>52.95135844927474</v>
       </c>
       <c r="E89" t="n">
-        <v>419.3160912523571</v>
+        <v>411.8155885141013</v>
       </c>
       <c r="F89" t="n">
         <v>1</v>
@@ -2227,79 +2227,79 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="B90" t="n">
-        <v>-255.28</v>
+        <v>164.52</v>
       </c>
       <c r="C90" t="n">
-        <v>5</v>
+        <v>-66.8</v>
       </c>
       <c r="D90" t="n">
-        <v>-26.12</v>
+        <v>-56.61</v>
       </c>
       <c r="E90" t="n">
-        <v>1064.339919849303</v>
+        <v>894.4560510744424</v>
       </c>
       <c r="F90" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B91" t="n">
-        <v>164.78</v>
+        <v>-115.18</v>
       </c>
       <c r="C91" t="n">
-        <v>-68</v>
+        <v>-25.25</v>
       </c>
       <c r="D91" t="n">
-        <v>-54.59</v>
+        <v>-36.27</v>
       </c>
       <c r="E91" t="n">
-        <v>933.4237342910632</v>
+        <v>554.9305468624422</v>
       </c>
       <c r="F91" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>2843404.369240924</v>
+        <v>416345.7451870226</v>
       </c>
       <c r="B92" t="n">
-        <v>79.430555865225</v>
+        <v>-100.1077717828337</v>
       </c>
       <c r="C92" t="n">
-        <v>-36.57172150508754</v>
+        <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>103.484187598182</v>
+        <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>505.6911551465355</v>
+        <v>459.6791802865195</v>
       </c>
       <c r="F92" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>3050</v>
+        <v>30500000</v>
       </c>
       <c r="B93" t="n">
-        <v>-109.94</v>
+        <v>-68.02</v>
       </c>
       <c r="C93" t="n">
-        <v>-19.62</v>
+        <v>70.73399999999999</v>
       </c>
       <c r="D93" t="n">
-        <v>-27.24</v>
+        <v>52.47</v>
       </c>
       <c r="E93" t="n">
-        <v>514.4037326287156</v>
+        <v>411.8827062807674</v>
       </c>
       <c r="F93" t="n">
         <v>1</v>
@@ -2327,19 +2327,19 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>35405.10211938623</v>
+        <v>530535.9455007528</v>
       </c>
       <c r="B95" t="n">
-        <v>-106.6663282582184</v>
+        <v>-99.49644958308151</v>
       </c>
       <c r="C95" t="n">
-        <v>-16.82913412914416</v>
+        <v>6.414739616791655</v>
       </c>
       <c r="D95" t="n">
-        <v>-21.53589196312405</v>
+        <v>4.221664161797348</v>
       </c>
       <c r="E95" t="n">
-        <v>487.1135065355699</v>
+        <v>456.9813219652531</v>
       </c>
       <c r="F95" t="n">
         <v>1</v>
@@ -2347,79 +2347,79 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>17995.07291338374</v>
+        <v>49044581.41950125</v>
       </c>
       <c r="B96" t="n">
-        <v>-100.257958624186</v>
+        <v>-85.37245149781344</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.8146995937526675</v>
+        <v>99.74914333659804</v>
       </c>
       <c r="D96" t="n">
-        <v>-1.131111974200952</v>
+        <v>61.74791677476886</v>
       </c>
       <c r="E96" t="n">
-        <v>494.6465526781491</v>
+        <v>893.4338440925756</v>
       </c>
       <c r="F96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>49044581.41950125</v>
+        <v>1</v>
       </c>
       <c r="B97" t="n">
-        <v>-85.37245149781344</v>
+        <v>-183.78</v>
       </c>
       <c r="C97" t="n">
-        <v>99.74914333659804</v>
+        <v>-65.5</v>
       </c>
       <c r="D97" t="n">
-        <v>61.74791677476886</v>
+        <v>-68.34</v>
       </c>
       <c r="E97" t="n">
-        <v>893.4338440925756</v>
+        <v>603.7072315371715</v>
       </c>
       <c r="F97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>20.70290093182177</v>
+        <v>2882822.168529236</v>
       </c>
       <c r="B98" t="n">
-        <v>-123.8712445521292</v>
+        <v>80.66367116761286</v>
       </c>
       <c r="C98" t="n">
-        <v>-31.96507525979762</v>
+        <v>-36.7564281141496</v>
       </c>
       <c r="D98" t="n">
-        <v>-48.04900907139718</v>
+        <v>101.9386502785829</v>
       </c>
       <c r="E98" t="n">
-        <v>569.977014103941</v>
+        <v>505.1441746011087</v>
       </c>
       <c r="F98" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>700</v>
+        <v>10.52250069864085</v>
       </c>
       <c r="B99" t="n">
-        <v>-112.206</v>
+        <v>-128.2225348049704</v>
       </c>
       <c r="C99" t="n">
-        <v>-20.62</v>
+        <v>-35.32699211184324</v>
       </c>
       <c r="D99" t="n">
-        <v>-31.24</v>
+        <v>-53.94619526298156</v>
       </c>
       <c r="E99" t="n">
-        <v>530.7866387564721</v>
+        <v>577.5100602465202</v>
       </c>
       <c r="F99" t="n">
         <v>1</v>
@@ -2427,19 +2427,19 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>335166.6920735188</v>
+        <v>4917315.128981112</v>
       </c>
       <c r="B100" t="n">
-        <v>-299.8130616203724</v>
+        <v>-254.6292588979523</v>
       </c>
       <c r="C100" t="n">
-        <v>66.00483771719875</v>
+        <v>78.42573861667788</v>
       </c>
       <c r="D100" t="n">
-        <v>35.79628572032509</v>
+        <v>54.9571417329734</v>
       </c>
       <c r="E100" t="n">
-        <v>961.5196576081412</v>
+        <v>924.8417097358416</v>
       </c>
       <c r="F100" t="n">
         <v>2</v>
@@ -2447,42 +2447,42 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>329549.1953043724</v>
+        <v>335166.6920735188</v>
       </c>
       <c r="B101" t="n">
-        <v>-100.515817291604</v>
+        <v>-299.8130616203724</v>
       </c>
       <c r="C101" t="n">
-        <v>0</v>
+        <v>66.00483771719875</v>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>35.79628572032509</v>
       </c>
       <c r="E101" t="n">
-        <v>462.2815195618131</v>
+        <v>961.5196576081412</v>
       </c>
       <c r="F101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>30774305.31316802</v>
+        <v>4920</v>
       </c>
       <c r="B102" t="n">
-        <v>-67.92178603266238</v>
+        <v>-261.07</v>
       </c>
       <c r="C102" t="n">
-        <v>70.45670458141744</v>
+        <v>8</v>
       </c>
       <c r="D102" t="n">
-        <v>52.79954833614673</v>
+        <v>-20.61</v>
       </c>
       <c r="E102" t="n">
-        <v>411.783045109778</v>
+        <v>1019.165107608548</v>
       </c>
       <c r="F102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>